<commit_message>
[fubo.ding] #115 bugfix: update tarv excel template
</commit_message>
<xml_diff>
--- a/src/main/resources/static/requisition/TARV_pt.xlsx
+++ b/src/main/resources/static/requisition/TARV_pt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubo.ding/projects_siglus_to14/siglus-api/src/main/resources/static/requisition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC87E31-49E2-954D-9B89-7D0D45782099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43B9471-6E20-C143-9BE4-38177FF6E2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37300" yWindow="-240" windowWidth="35840" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TARV" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="146">
   <si>
     <r>
       <rPr>
@@ -341,12 +341,6 @@
     <t>Ajuste</t>
   </si>
   <si>
-    <t>Visto por:</t>
-  </si>
-  <si>
-    <t>Data de elaboração:</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -494,22 +488,6 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Elaborado por:</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>{authorize}</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>{approve}</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
-    <t>{createdDate}</t>
-    <phoneticPr fontId="10" type="noConversion"/>
-  </si>
-  <si>
     <t>Novos</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -711,6 +689,22 @@
   </si>
   <si>
     <t>{totalTotal}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Elaborado por:{authorize}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Visto por:{approve}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data de elaboração:{createdDate}</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>{comment}</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -843,7 +837,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1072,11 +1066,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1219,104 +1222,125 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1745,16 +1769,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" customWidth="1"/>
     <col min="3" max="3" width="55.796875" customWidth="1"/>
-    <col min="4" max="4" width="16.796875" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="28.19921875" customWidth="1"/>
@@ -1765,66 +1789,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="41.75" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="56" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
       <c r="I1" s="25" t="s">
         <v>30</v>
       </c>
       <c r="J1" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="14.5" customHeight="1">
-      <c r="A2" s="70"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="74" t="s">
+      <c r="C2" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="72" t="s">
-        <v>61</v>
+      <c r="J2" s="59" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" customHeight="1">
-      <c r="A3" s="71"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="73"/>
+      <c r="E3" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="1:13" ht="29.5" customHeight="1">
       <c r="A4" s="40"/>
@@ -1858,34 +1882,34 @@
     </row>
     <row r="5" spans="1:13" ht="34" customHeight="1">
       <c r="A5" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="E5" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="F5" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="G5" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="H5" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="I5" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="J5" s="34" t="s">
         <v>70</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="K5" s="35"/>
     </row>
@@ -1896,39 +1920,39 @@
     </row>
     <row r="7" spans="1:13" ht="12.75" customHeight="1">
       <c r="A7" s="40"/>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="54" t="s">
+      <c r="C7" s="68"/>
+      <c r="D7" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
     <row r="8" spans="1:13" ht="25" customHeight="1">
       <c r="A8" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>76</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -1937,7 +1961,7 @@
     </row>
     <row r="9" spans="1:13" ht="12.75" customHeight="1">
       <c r="A9" s="40"/>
-      <c r="B9" s="55"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="14"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -1948,7 +1972,7 @@
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1">
       <c r="A10" s="40"/>
-      <c r="B10" s="55"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="14"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -1959,19 +1983,19 @@
     </row>
     <row r="11" spans="1:13" ht="25" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="52" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="34" t="s">
         <v>77</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E11" s="34" t="s">
-        <v>79</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1980,7 +2004,7 @@
     </row>
     <row r="12" spans="1:13" ht="12.25" customHeight="1">
       <c r="A12" s="40"/>
-      <c r="B12" s="56"/>
+      <c r="B12" s="55"/>
       <c r="C12" s="15"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1991,7 +2015,7 @@
     </row>
     <row r="13" spans="1:13" ht="13" customHeight="1">
       <c r="A13" s="40"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="15"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
@@ -2007,10 +2031,10 @@
         <v>8</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -2032,15 +2056,15 @@
       <c r="A16" s="40">
         <v>1</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="66"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
@@ -2051,15 +2075,15 @@
       <c r="A17" s="40">
         <v>2</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="66"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -2070,15 +2094,15 @@
       <c r="A18" s="40">
         <v>3</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="66"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
@@ -2092,10 +2116,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -2103,496 +2127,501 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" ht="14" customHeight="1"/>
-    <row r="21" spans="1:10" s="46" customFormat="1" ht="24" customHeight="1">
+    <row r="21" spans="1:10" s="46" customFormat="1" ht="35" customHeight="1">
       <c r="B21" s="47" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="C21" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="49"/>
-      <c r="G21" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>96</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="D21" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="78"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
     </row>
     <row r="22" spans="1:10" ht="14" customHeight="1"/>
     <row r="23" spans="1:10" ht="14" customHeight="1">
-      <c r="G23" s="65" t="s">
+      <c r="B23" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="84"/>
+      <c r="E23" s="84"/>
     </row>
     <row r="24" spans="1:10" ht="14" customHeight="1">
-      <c r="G24" s="59" t="s">
+      <c r="B24" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="13" customHeight="1">
+      <c r="B25" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="13" customHeight="1">
+      <c r="B26" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="80"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="13" customHeight="1">
+      <c r="B27" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="H24" s="60"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="4" t="s">
+      <c r="C27" s="80"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
-      <c r="G25" s="64" t="s">
+    <row r="28" spans="1:10" ht="13" customHeight="1">
+      <c r="B28" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="4" t="s">
+      <c r="C28" s="80"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
-      <c r="G26" s="64" t="s">
+    <row r="29" spans="1:10" ht="14" customHeight="1">
+      <c r="B29" s="82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="83"/>
+      <c r="D29" s="83"/>
+      <c r="E29" s="83"/>
+    </row>
+    <row r="30" spans="1:10" ht="13" customHeight="1">
+      <c r="B30" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="H26" s="60"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="4" t="s">
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="13" customHeight="1">
-      <c r="G27" s="64" t="s">
+    <row r="31" spans="1:10" ht="13" customHeight="1">
+      <c r="B31" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="H27" s="60"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="4" t="s">
+      <c r="C31" s="80"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
-      <c r="G28" s="64" t="s">
+    <row r="32" spans="1:10" ht="13" customHeight="1">
+      <c r="B32" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="70"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="60"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="4" t="s">
+    </row>
+    <row r="33" spans="2:7" ht="13" customHeight="1">
+      <c r="B33" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="70"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14" customHeight="1">
-      <c r="G29" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="63"/>
-      <c r="I29" s="63"/>
-      <c r="J29" s="63"/>
-    </row>
-    <row r="30" spans="1:10" ht="13" customHeight="1">
-      <c r="G30" s="64" t="s">
+    <row r="34" spans="2:7" ht="13" customHeight="1">
+      <c r="B34" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="86"/>
+      <c r="D34" s="86"/>
+      <c r="E34" s="86"/>
+    </row>
+    <row r="35" spans="2:7" ht="13" customHeight="1">
+      <c r="B35" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="H30" s="60"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="4" t="s">
+      <c r="C35" s="80"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="13" customHeight="1">
-      <c r="G31" s="64" t="s">
+    <row r="36" spans="2:7" ht="13" customHeight="1">
+      <c r="B36" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="H31" s="60"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="4" t="s">
+      <c r="C36" s="80"/>
+      <c r="D36" s="81"/>
+      <c r="E36" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="13" customHeight="1">
-      <c r="G32" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32" s="60"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="4" t="s">
+    <row r="37" spans="2:7" ht="13" customHeight="1">
+      <c r="B37" s="85" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+    </row>
+    <row r="38" spans="2:7" ht="13" customHeight="1">
+      <c r="B38" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="7:12" ht="13" customHeight="1">
-      <c r="G33" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="60"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="4" t="s">
+    <row r="39" spans="2:7" ht="13" customHeight="1">
+      <c r="B39" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="70"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="7:12" ht="13" customHeight="1">
-      <c r="G34" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
-    </row>
-    <row r="35" spans="7:12" ht="13" customHeight="1">
-      <c r="G35" s="64" t="s">
+    <row r="40" spans="2:7" ht="13" customHeight="1">
+      <c r="B40" s="82" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="83"/>
+      <c r="D40" s="83"/>
+      <c r="E40" s="83"/>
+    </row>
+    <row r="41" spans="2:7" ht="13" customHeight="1">
+      <c r="B41" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="70"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H35" s="60"/>
-      <c r="I35" s="61"/>
-      <c r="J35" s="4" t="s">
+    </row>
+    <row r="42" spans="2:7" ht="13" customHeight="1">
+      <c r="B42" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="70"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="7:12" ht="13" customHeight="1">
-      <c r="G36" s="64" t="s">
+    <row r="43" spans="2:7" ht="13" customHeight="1">
+      <c r="B43" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="80"/>
+      <c r="D43" s="81"/>
+      <c r="E43" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H36" s="60"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="4" t="s">
+    </row>
+    <row r="44" spans="2:7" ht="13" customHeight="1">
+      <c r="B44" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="70"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="7:12" ht="13" customHeight="1">
-      <c r="G37" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="63"/>
-    </row>
-    <row r="38" spans="7:12" ht="13" customHeight="1">
-      <c r="G38" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="H38" s="60"/>
-      <c r="I38" s="61"/>
-      <c r="J38" s="4" t="s">
+    <row r="45" spans="2:7" ht="13" customHeight="1">
+      <c r="B45" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="70"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="7:12" ht="13" customHeight="1">
-      <c r="G39" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="H39" s="60"/>
-      <c r="I39" s="61"/>
-      <c r="J39" s="4" t="s">
+    <row r="46" spans="2:7" ht="13" customHeight="1">
+      <c r="B46" s="85" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+    </row>
+    <row r="47" spans="2:7" ht="13" customHeight="1">
+      <c r="B47" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="70"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="7:12" ht="13" customHeight="1">
-      <c r="G40" s="65" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="63"/>
-      <c r="I40" s="63"/>
-      <c r="J40" s="63"/>
-    </row>
-    <row r="41" spans="7:12" ht="13" customHeight="1">
-      <c r="G41" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="H41" s="60"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="4" t="s">
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="2:7" ht="13" customHeight="1">
+      <c r="B48" s="69" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="70"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="7:12" ht="13" customHeight="1">
-      <c r="G42" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="60"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="4" t="s">
+      <c r="F48" s="16"/>
+    </row>
+    <row r="49" spans="2:12" ht="13" customHeight="1">
+      <c r="B49" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="80"/>
+      <c r="D49" s="81"/>
+      <c r="E49" s="49" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="7:12" ht="13" customHeight="1">
-      <c r="G43" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="H43" s="60"/>
-      <c r="I43" s="61"/>
-      <c r="J43" s="4" t="s">
+      <c r="G49" s="2"/>
+    </row>
+    <row r="50" spans="2:12" ht="13" customHeight="1">
+      <c r="B50" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="70"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="44" spans="7:12" ht="13" customHeight="1">
-      <c r="G44" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="H44" s="60"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="4" t="s">
+    <row r="51" spans="2:12" ht="13" customHeight="1">
+      <c r="B51" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="80"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="45" spans="7:12" ht="13" customHeight="1">
-      <c r="G45" s="59" t="s">
+    <row r="52" spans="2:12" ht="13" customHeight="1"/>
+    <row r="53" spans="2:12" ht="13" customHeight="1">
+      <c r="B53" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
+    </row>
+    <row r="54" spans="2:12" ht="13" customHeight="1">
+      <c r="B54" s="44"/>
+      <c r="C54" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="14">
+      <c r="B55" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="14" customHeight="1">
+      <c r="B56" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="57" spans="2:12" ht="14" customHeight="1">
+      <c r="B57" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="17"/>
+    </row>
+    <row r="58" spans="2:12" ht="14">
+      <c r="B58" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E58" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" s="8"/>
+      <c r="G58" s="17"/>
+    </row>
+    <row r="59" spans="2:12" ht="14" customHeight="1">
+      <c r="B59" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E59" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G59" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H45" s="60"/>
-      <c r="I45" s="61"/>
-      <c r="J45" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="7:12" ht="13" customHeight="1">
-      <c r="G46" s="62" t="s">
-        <v>25</v>
-      </c>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-    </row>
-    <row r="47" spans="7:12" ht="13" customHeight="1">
-      <c r="G47" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" s="60"/>
-      <c r="I47" s="61"/>
-      <c r="J47" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="7:12" ht="13" customHeight="1">
-      <c r="G48" s="59" t="s">
-        <v>10</v>
-      </c>
-      <c r="H48" s="60"/>
-      <c r="I48" s="61"/>
-      <c r="J48" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="K48" s="16"/>
-    </row>
-    <row r="49" spans="7:12" ht="13" customHeight="1">
-      <c r="G49" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="H49" s="60"/>
-      <c r="I49" s="61"/>
-      <c r="J49" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="L49" s="2"/>
-    </row>
-    <row r="50" spans="7:12" ht="13" customHeight="1">
-      <c r="G50" s="59" t="s">
-        <v>11</v>
-      </c>
-      <c r="H50" s="60"/>
-      <c r="I50" s="61"/>
-      <c r="J50" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="7:12" ht="13" customHeight="1">
-      <c r="G51" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="H51" s="60"/>
-      <c r="I51" s="61"/>
-      <c r="J51" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="7:12" ht="13" customHeight="1"/>
-    <row r="53" spans="7:12" ht="13" customHeight="1">
-      <c r="G53" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
-      <c r="J53" s="58"/>
-      <c r="K53" s="58"/>
-      <c r="L53" s="58"/>
-    </row>
-    <row r="54" spans="7:12" ht="13" customHeight="1">
-      <c r="G54" s="44"/>
-      <c r="H54" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="7:12" ht="14">
-      <c r="G55" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="H55" s="42" t="s">
+    </row>
+    <row r="60" spans="2:12" ht="14">
+      <c r="B60" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="G60" s="50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="14" customHeight="1">
+      <c r="B61" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="I55" s="7"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
-      <c r="L55" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="7:12" ht="14" customHeight="1">
-      <c r="G56" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="H56" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="I56" s="8"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="17"/>
-    </row>
-    <row r="57" spans="7:12" ht="14" customHeight="1">
-      <c r="G57" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="H57" s="42" t="s">
+      <c r="D61" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="I57" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J57" s="7"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="17"/>
-    </row>
-    <row r="58" spans="7:12" ht="14">
-      <c r="G58" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="H58" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="J58" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="K58" s="8"/>
-      <c r="L58" s="17"/>
-    </row>
-    <row r="59" spans="7:12" ht="14" customHeight="1">
-      <c r="G59" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="H59" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="I59" s="42" t="s">
+      <c r="E61" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F61" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="J59" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="K59" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="L59" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="7:12" ht="14">
-      <c r="G60" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="H60" s="42" t="s">
-        <v>135</v>
-      </c>
-      <c r="I60" s="42" t="s">
-        <v>140</v>
-      </c>
-      <c r="J60" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="K60" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="L60" s="51" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="7:12" ht="14" customHeight="1">
-      <c r="G61" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H61" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="I61" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="J61" s="21" t="s">
+      <c r="G61" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="K61" s="21" t="s">
+    </row>
+    <row r="63" spans="2:12" ht="13" customHeight="1">
+      <c r="B63" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="L61" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="7:12" ht="13" customHeight="1"/>
-    <row r="64" spans="7:12" ht="16" customHeight="1">
+      <c r="C63" s="79"/>
+      <c r="D63" s="79"/>
+      <c r="E63" s="79"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="79"/>
+    </row>
+    <row r="64" spans="2:12" ht="16" customHeight="1">
       <c r="K64" s="38"/>
       <c r="L64" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="43">
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="B63:G63"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="C2:H2"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G53:L53"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G40:J40"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>